<commit_message>
Login and log out buttons
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GUSTAV\source\repos\EVEDRI_Lab_Act2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ACT-STUDENT\source\repos\EVEDRI_Lab_Act2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C7F9D31-CFA4-424F-B52E-1EDCD668D87C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6D63390-C462-4B10-A866-D24CC128F4ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RECORDS" sheetId="1" r:id="rId1"/>
@@ -551,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB32F544-3CFA-40B4-90DD-B147A743AC79}">
   <dimension ref="A1:N4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M15" sqref="M15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,9 +736,6 @@
       <c r="L4" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M4">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -754,7 +751,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BBE2ECA-D8E0-46A9-8305-09FFCE3338AA}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
buttons for act and inact in progress
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="89">
   <si>
     <t>Name</t>
   </si>
@@ -120,30 +120,30 @@
     <t>Profile</t>
   </si>
   <si>
+    <t>https://www.e-iceblue.com/Buy/Spire.XLS.html</t>
+  </si>
+  <si>
+    <t>Buy Now!</t>
+  </si>
+  <si>
+    <t>mailto:support@e-iceblue.com</t>
+  </si>
+  <si>
+    <t>Contact US</t>
+  </si>
+  <si>
+    <t>https://www.e-iceblue.com</t>
+  </si>
+  <si>
+    <t>Home page</t>
+  </si>
+  <si>
+    <t>e-iceblue Inc. 2002-2025 All rights reserverd</t>
+  </si>
+  <si>
     <t>Spire.XLS for .NET</t>
   </si>
   <si>
-    <t>e-iceblue Inc. 2002-2025 All rights reserverd</t>
-  </si>
-  <si>
-    <t>Home page</t>
-  </si>
-  <si>
-    <t>https://www.e-iceblue.com</t>
-  </si>
-  <si>
-    <t>Contact US</t>
-  </si>
-  <si>
-    <t>mailto:support@e-iceblue.com</t>
-  </si>
-  <si>
-    <t>Buy Now!</t>
-  </si>
-  <si>
-    <t>https://www.e-iceblue.com/Buy/Spire.XLS.html</t>
-  </si>
-  <si>
     <t>C:\Users\GUSTAV\source\repos\EVEDRI_Lab_Act2\EVEDRI_Lab_Act2\Pictures\Avatar 1.jpg</t>
   </si>
   <si>
@@ -208,6 +208,87 @@
   </si>
   <si>
     <t>Successfully Logged Out!</t>
+  </si>
+  <si>
+    <t>Added new user: spam</t>
+  </si>
+  <si>
+    <t>Added new user: asdfmdhgnfdvcs</t>
+  </si>
+  <si>
+    <t>kl.kl.kl.</t>
+  </si>
+  <si>
+    <t>Added new user: dk.kl.lk.kl.kl.</t>
+  </si>
+  <si>
+    <t>kgbvbxcv</t>
+  </si>
+  <si>
+    <t>Added new user: kgbvbxcv</t>
+  </si>
+  <si>
+    <t>spam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volleyball, </t>
+  </si>
+  <si>
+    <t>asdasghjkl;</t>
+  </si>
+  <si>
+    <t>dvxzcgnbty dsdfr</t>
+  </si>
+  <si>
+    <t>vadfsgbvtrbrbdf</t>
+  </si>
+  <si>
+    <t>dasdasd</t>
+  </si>
+  <si>
+    <t>asdsdgfvf vf</t>
+  </si>
+  <si>
+    <t>asdasdasd</t>
+  </si>
+  <si>
+    <t>trbdfbtr</t>
+  </si>
+  <si>
+    <t>Added new user: asdasghjkl;</t>
+  </si>
+  <si>
+    <t>asdsgtrbtynbyd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Basketball, </t>
+  </si>
+  <si>
+    <t>tvafggegntfmdsdq</t>
+  </si>
+  <si>
+    <t>hdxfdsFGEHB</t>
+  </si>
+  <si>
+    <t>yjmio,oi,</t>
+  </si>
+  <si>
+    <t>sdcasdbwev hyt</t>
+  </si>
+  <si>
+    <t>SHVYDTBHNN SF</t>
+  </si>
+  <si>
+    <t>DFXCHYBRGB</t>
+  </si>
+  <si>
+    <t>Added new user: asdsgtrbtynbyd</t>
+  </si>
+  <si>
+    <t>Deleted an active student</t>
+  </si>
+  <si>
+    <t>Deleted an inactive user</t>
   </si>
 </sst>
 </file>
@@ -280,7 +361,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="399">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -304,9 +385,387 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -323,7 +782,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="20" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="398" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -339,8 +798,12 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="20"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="398"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0"/>
@@ -349,7 +812,7 @@
     <cellStyle name="Currency [0]" xfId="17"/>
     <cellStyle name="Comma" xfId="18"/>
     <cellStyle name="Comma [0]" xfId="19"/>
-    <cellStyle name="Hyperlink" xfId="20"/>
+    <cellStyle name="Hyperlink" xfId="398"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -728,10 +1191,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB32F544-3CFA-40B4-90DD-B147A743AC79}">
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="E1">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1060,6 +1523,138 @@
         <v>1</v>
       </c>
     </row>
+    <row r="8" spans="1:14" ht="15">
+      <c r="A8" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" t="s">
+        <v>68</v>
+      </c>
+      <c r="F8" t="s">
+        <v>68</v>
+      </c>
+      <c r="G8" s="17">
+        <v>34833</v>
+      </c>
+      <c r="H8" s="4">
+        <v>30</v>
+      </c>
+      <c r="I8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J8" t="s">
+        <v>68</v>
+      </c>
+      <c r="K8" t="s">
+        <v>68</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" t="s">
+        <v>68</v>
+      </c>
+      <c r="N8" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="15">
+      <c r="A9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D9" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" s="17">
+        <v>34833</v>
+      </c>
+      <c r="H9" s="4">
+        <v>30</v>
+      </c>
+      <c r="I9" t="s">
+        <v>73</v>
+      </c>
+      <c r="J9" t="s">
+        <v>74</v>
+      </c>
+      <c r="K9" t="s">
+        <v>75</v>
+      </c>
+      <c r="L9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9" t="s">
+        <v>76</v>
+      </c>
+      <c r="N9" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="15">
+      <c r="A10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>79</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F10" t="s">
+        <v>81</v>
+      </c>
+      <c r="G10" s="17">
+        <v>34833</v>
+      </c>
+      <c r="H10" s="4">
+        <v>30</v>
+      </c>
+      <c r="I10" t="s">
+        <v>82</v>
+      </c>
+      <c r="J10" t="s">
+        <v>83</v>
+      </c>
+      <c r="K10" t="s">
+        <v>84</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" t="s">
+        <v>85</v>
+      </c>
+      <c r="N10" s="4">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="F3" r:id="rId1" display="mailto:sad@test.com"/>
@@ -1073,7 +1668,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BBE2ECA-D8E0-46A9-8305-09FFCE3338AA}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A1">
       <selection activeCell="A30" sqref="A30"/>
@@ -1659,6 +2254,501 @@
       </c>
       <c r="D41" s="14">
         <v>45788.978090277778</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="15">
+      <c r="A42" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B42" t="s">
+        <v>60</v>
+      </c>
+      <c r="C42" s="14">
+        <v>45791</v>
+      </c>
+      <c r="D42" s="14">
+        <v>45791.700601851851</v>
+      </c>
+    </row>
+    <row r="43" spans="2:4" ht="15">
+      <c r="B43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C43" s="14">
+        <v>45791</v>
+      </c>
+      <c r="D43" s="14">
+        <v>45791.700995370367</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="15">
+      <c r="A44" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B44" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" s="14">
+        <v>45791</v>
+      </c>
+      <c r="D44" s="14">
+        <v>45791.701354166667</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="15">
+      <c r="A45" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B45" t="s">
+        <v>60</v>
+      </c>
+      <c r="C45" s="14">
+        <v>45791</v>
+      </c>
+      <c r="D45" s="14">
+        <v>45791.702268518522</v>
+      </c>
+    </row>
+    <row r="46" spans="2:4" ht="15">
+      <c r="B46" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" s="14">
+        <v>45791</v>
+      </c>
+      <c r="D46" s="14">
+        <v>45791.702569444446</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="15">
+      <c r="A47" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47" t="s">
+        <v>61</v>
+      </c>
+      <c r="C47" s="14">
+        <v>45791</v>
+      </c>
+      <c r="D47" s="14">
+        <v>45791.702905092592</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="15">
+      <c r="A48" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B48" t="s">
+        <v>60</v>
+      </c>
+      <c r="C48" s="14">
+        <v>45791</v>
+      </c>
+      <c r="D48" s="14">
+        <v>45791.70385416667</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15">
+      <c r="A49" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B49" t="s">
+        <v>65</v>
+      </c>
+      <c r="C49" s="14">
+        <v>45791</v>
+      </c>
+      <c r="D49" s="14">
+        <v>45791.704189814816</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="15">
+      <c r="A50" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B50" t="s">
+        <v>60</v>
+      </c>
+      <c r="C50" s="14">
+        <v>45791</v>
+      </c>
+      <c r="D50" s="14">
+        <v>45791.706782407404</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="15">
+      <c r="A51" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" s="14">
+        <v>45791</v>
+      </c>
+      <c r="D51" s="14">
+        <v>45791.707025462965</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="15">
+      <c r="A52" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B52" t="s">
+        <v>60</v>
+      </c>
+      <c r="C52" s="14">
+        <v>45791</v>
+      </c>
+      <c r="D52" s="14">
+        <v>45791.708067129628</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="15">
+      <c r="A53" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B53" t="s">
+        <v>61</v>
+      </c>
+      <c r="C53" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D53" s="15">
+        <v>45791.708877314813</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" ht="15">
+      <c r="A54" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B54" t="s">
+        <v>60</v>
+      </c>
+      <c r="C54" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D54" s="15">
+        <v>45791.70894675926</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="15">
+      <c r="A55" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D55" s="15">
+        <v>45791.709340277775</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="15">
+      <c r="A56" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B56" t="s">
+        <v>61</v>
+      </c>
+      <c r="C56" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D56" s="15">
+        <v>45791.7103125</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="15">
+      <c r="A57" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" t="s">
+        <v>60</v>
+      </c>
+      <c r="C57" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D57" s="15">
+        <v>45791.711041666669</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" ht="15">
+      <c r="B58" t="s">
+        <v>77</v>
+      </c>
+      <c r="C58" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D58" s="15">
+        <v>45791.712245370371</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="15">
+      <c r="A59" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B59" t="s">
+        <v>61</v>
+      </c>
+      <c r="C59" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D59" s="15">
+        <v>45791.715173611112</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="15">
+      <c r="A60" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B60" t="s">
+        <v>60</v>
+      </c>
+      <c r="C60" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D60" s="15">
+        <v>45791.716527777775</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="15">
+      <c r="A61" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61" t="s">
+        <v>86</v>
+      </c>
+      <c r="C61" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D61" s="15">
+        <v>45791.716840277775</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="15">
+      <c r="A62" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B62" t="s">
+        <v>61</v>
+      </c>
+      <c r="C62" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D62" s="15">
+        <v>45791.729432870372</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="15">
+      <c r="A63" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B63" t="s">
+        <v>60</v>
+      </c>
+      <c r="C63" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D63" s="15">
+        <v>45791.750185185185</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="15">
+      <c r="A64" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B64" t="s">
+        <v>61</v>
+      </c>
+      <c r="C64" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D64" s="15">
+        <v>45791.750277777777</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="15">
+      <c r="A65" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B65" t="s">
+        <v>60</v>
+      </c>
+      <c r="C65" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D65" s="15">
+        <v>45791.750358796293</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="15">
+      <c r="A66" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B66" t="s">
+        <v>61</v>
+      </c>
+      <c r="C66" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D66" s="15">
+        <v>45791.750405092593</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" ht="15">
+      <c r="A67" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B67" t="s">
+        <v>60</v>
+      </c>
+      <c r="C67" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D67" s="15">
+        <v>45791.750879629632</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="15">
+      <c r="A68" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B68" t="s">
+        <v>61</v>
+      </c>
+      <c r="C68" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D68" s="15">
+        <v>45791.7512037037</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="15">
+      <c r="A69" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B69" t="s">
+        <v>60</v>
+      </c>
+      <c r="C69" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D69" s="15">
+        <v>45791.751423611109</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="15">
+      <c r="A70" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B70" t="s">
+        <v>61</v>
+      </c>
+      <c r="C70" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D70" s="15">
+        <v>45791.752893518518</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="15">
+      <c r="A71" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B71" t="s">
+        <v>60</v>
+      </c>
+      <c r="C71" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D71" s="15">
+        <v>45791.759664351855</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="15">
+      <c r="A72" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B72" t="s">
+        <v>87</v>
+      </c>
+      <c r="C72" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D72" s="15">
+        <v>45791.759756944448</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="15">
+      <c r="A73" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B73" t="s">
+        <v>88</v>
+      </c>
+      <c r="C73" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D73" s="15">
+        <v>45791.759791666664</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="15">
+      <c r="A74" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B74" t="s">
+        <v>60</v>
+      </c>
+      <c r="C74" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D74" s="15">
+        <v>45791.769571759258</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="15">
+      <c r="A75" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B75" t="s">
+        <v>87</v>
+      </c>
+      <c r="C75" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D75" s="15">
+        <v>45791.769953703704</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="15">
+      <c r="A76" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B76" t="s">
+        <v>87</v>
+      </c>
+      <c r="C76" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D76" s="15">
+        <v>45791.770208333335</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="15">
+      <c r="A77" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B77" t="s">
+        <v>61</v>
+      </c>
+      <c r="C77" s="15">
+        <v>45791</v>
+      </c>
+      <c r="D77" s="15">
+        <v>45791.770868055559</v>
       </c>
     </row>
   </sheetData>
@@ -1678,42 +2768,42 @@
   <sheetData>
     <row r="1" ht="15">
       <c r="B1" s="8" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" ht="15">
       <c r="B2" s="8" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" ht="15">
       <c r="B4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" ht="15">
       <c r="B5" s="9" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="7" ht="15">
       <c r="B7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" ht="15">
       <c r="B8" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" ht="15">
       <c r="B10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" ht="15">
       <c r="B11" s="9" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed the count of inactive
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="102">
   <si>
     <t>Name</t>
   </si>
@@ -400,7 +400,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="399">
+  <cellStyleXfs count="665">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment/>
       <protection/>
@@ -424,6 +424,272 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -821,7 +1087,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="398" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="664" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -843,7 +1109,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="398"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="664"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Normal" xfId="0"/>
@@ -852,7 +1118,7 @@
     <cellStyle name="Currency [0]" xfId="17"/>
     <cellStyle name="Comma" xfId="18"/>
     <cellStyle name="Comma [0]" xfId="19"/>
-    <cellStyle name="Hyperlink" xfId="398"/>
+    <cellStyle name="Hyperlink" xfId="664"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -1604,7 +1870,7 @@
         <v>41</v>
       </c>
       <c r="N8" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="15">
@@ -1708,7 +1974,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BBE2ECA-D8E0-46A9-8305-09FFCE3338AA}">
-  <dimension ref="A1:D150"/>
+  <dimension ref="A1:D163"/>
   <sheetViews>
     <sheetView workbookViewId="0" topLeftCell="A16">
       <selection activeCell="A30" sqref="A30"/>
@@ -3811,6 +4077,188 @@
       </c>
       <c r="D150" s="17">
         <v>45792.131284722222</v>
+      </c>
+    </row>
+    <row r="151" spans="1:4" ht="15">
+      <c r="A151" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B151" t="s">
+        <v>60</v>
+      </c>
+      <c r="C151" s="17">
+        <v>45792</v>
+      </c>
+      <c r="D151" s="17">
+        <v>45792.137465277781</v>
+      </c>
+    </row>
+    <row r="152" spans="1:4" ht="15">
+      <c r="A152" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B152" t="s">
+        <v>87</v>
+      </c>
+      <c r="C152" s="17">
+        <v>45792</v>
+      </c>
+      <c r="D152" s="17">
+        <v>45792.13758101852</v>
+      </c>
+    </row>
+    <row r="153" spans="1:4" ht="15">
+      <c r="A153" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B153" t="s">
+        <v>88</v>
+      </c>
+      <c r="C153" s="17">
+        <v>45792</v>
+      </c>
+      <c r="D153" s="17">
+        <v>45792.13758101852</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" ht="15">
+      <c r="A154" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B154" t="s">
+        <v>97</v>
+      </c>
+      <c r="C154" s="17">
+        <v>45792</v>
+      </c>
+      <c r="D154" s="17">
+        <v>45792.137881944444</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" ht="15">
+      <c r="A155" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B155" t="s">
+        <v>98</v>
+      </c>
+      <c r="C155" s="17">
+        <v>45792</v>
+      </c>
+      <c r="D155" s="17">
+        <v>45792.137881944444</v>
+      </c>
+    </row>
+    <row r="156" spans="1:4" ht="15">
+      <c r="A156" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B156" t="s">
+        <v>100</v>
+      </c>
+      <c r="C156" s="17">
+        <v>45792</v>
+      </c>
+      <c r="D156" s="17">
+        <v>45792.137881944444</v>
+      </c>
+    </row>
+    <row r="157" spans="1:4" ht="15">
+      <c r="A157" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B157" t="s">
+        <v>87</v>
+      </c>
+      <c r="C157" s="17">
+        <v>45792</v>
+      </c>
+      <c r="D157" s="17">
+        <v>45792.138009259259</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" ht="15">
+      <c r="A158" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B158" t="s">
+        <v>60</v>
+      </c>
+      <c r="C158" s="17">
+        <v>45792</v>
+      </c>
+      <c r="D158" s="17">
+        <v>45792.138877314814</v>
+      </c>
+    </row>
+    <row r="159" spans="1:4" ht="15">
+      <c r="A159" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B159" t="s">
+        <v>88</v>
+      </c>
+      <c r="C159" s="17">
+        <v>45792</v>
+      </c>
+      <c r="D159" s="17">
+        <v>45792.138993055552</v>
+      </c>
+    </row>
+    <row r="160" spans="1:4" ht="15">
+      <c r="A160" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B160" t="s">
+        <v>90</v>
+      </c>
+      <c r="C160" s="17">
+        <v>45792</v>
+      </c>
+      <c r="D160" s="17">
+        <v>45792.139155092591</v>
+      </c>
+    </row>
+    <row r="161" spans="1:4" ht="15">
+      <c r="A161" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B161" t="s">
+        <v>101</v>
+      </c>
+      <c r="C161" s="17">
+        <v>45792</v>
+      </c>
+      <c r="D161" s="17">
+        <v>45792.139155092591</v>
+      </c>
+    </row>
+    <row r="162" spans="1:4" ht="15">
+      <c r="A162" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B162" t="s">
+        <v>97</v>
+      </c>
+      <c r="C162" s="17">
+        <v>45792</v>
+      </c>
+      <c r="D162" s="17">
+        <v>45792.139270833337</v>
+      </c>
+    </row>
+    <row r="163" spans="1:4" ht="15">
+      <c r="A163" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B163" t="s">
+        <v>98</v>
+      </c>
+      <c r="C163" s="17">
+        <v>45792</v>
+      </c>
+      <c r="D163" s="17">
+        <v>45792.139270833337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>